<commit_message>
ready for data collection
</commit_message>
<xml_diff>
--- a/pa1/bound.xlsx
+++ b/pa1/bound.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="260" yWindow="100" windowWidth="27160" windowHeight="14140"/>
+    <workbookView xWindow="255" yWindow="105" windowWidth="27165" windowHeight="14145"/>
   </bookViews>
   <sheets>
     <sheet name="r0" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -591,40 +591,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32.0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>64.0</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>128.0</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>256.0</c:v>
+                  <c:v>256</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>512.0</c:v>
+                  <c:v>512</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1024.0</c:v>
+                  <c:v>1024</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2048.0</c:v>
+                  <c:v>2048</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4096.0</c:v>
+                  <c:v>4096</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8192.0</c:v>
+                  <c:v>8192</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>16384.0</c:v>
+                  <c:v>16384</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>32678.0</c:v>
+                  <c:v>32678</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -639,37 +639,37 @@
                   <c:v>0.244588</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.151885</c:v>
+                  <c:v>0.15188499999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.08949</c:v>
+                  <c:v>8.949E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.046354</c:v>
+                  <c:v>4.6353999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.03302</c:v>
+                  <c:v>3.3020000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.013119</c:v>
+                  <c:v>1.3119E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.008268</c:v>
+                  <c:v>8.2679999999999993E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.005599</c:v>
+                  <c:v>5.5989999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.002211</c:v>
+                  <c:v>2.2109999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.001533</c:v>
+                  <c:v>1.5330000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.000749</c:v>
+                  <c:v>7.4899999999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.000371</c:v>
+                  <c:v>3.7100000000000002E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -680,7 +680,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>1/log(n)</c:v>
+            <c:v>1.5/log(n)-.09</c:v>
           </c:tx>
           <c:marker>
             <c:symbol val="none"/>
@@ -692,40 +692,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32.0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>64.0</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>128.0</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>256.0</c:v>
+                  <c:v>256</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>512.0</c:v>
+                  <c:v>512</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1024.0</c:v>
+                  <c:v>1024</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2048.0</c:v>
+                  <c:v>2048</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4096.0</c:v>
+                  <c:v>4096</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8192.0</c:v>
+                  <c:v>8192</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>16384.0</c:v>
+                  <c:v>16384</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>32678.0</c:v>
+                  <c:v>32678</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -737,40 +737,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0.25</c:v>
+                  <c:v>0.28500000000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.2</c:v>
+                  <c:v>0.21</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.166666666666667</c:v>
+                  <c:v>0.16</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.142857142857143</c:v>
+                  <c:v>0.12428571428571428</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.125</c:v>
+                  <c:v>9.7500000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.111111111111111</c:v>
+                  <c:v>7.6666666666666661E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.1</c:v>
+                  <c:v>0.06</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.0909090909090909</c:v>
+                  <c:v>4.6363636363636357E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.0833333333333333</c:v>
+                  <c:v>3.5000000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.0769230769230769</c:v>
+                  <c:v>2.5384615384615394E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.0714285714285714</c:v>
+                  <c:v>1.714285714285714E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.0666843065858174</c:v>
+                  <c:v>1.0026459878726121E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -787,11 +787,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="552933896"/>
-        <c:axId val="553435512"/>
+        <c:axId val="38996992"/>
+        <c:axId val="109841792"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="552933896"/>
+        <c:axId val="38996992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -801,7 +801,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="553435512"/>
+        <c:crossAx val="109841792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -809,7 +809,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="553435512"/>
+        <c:axId val="109841792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -820,7 +820,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="552933896"/>
+        <c:crossAx val="38996992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -836,7 +836,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -878,40 +878,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32.0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>64.0</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>128.0</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>256.0</c:v>
+                  <c:v>256</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>512.0</c:v>
+                  <c:v>512</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1024.0</c:v>
+                  <c:v>1024</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2048.0</c:v>
+                  <c:v>2048</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4096.0</c:v>
+                  <c:v>4096</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8192.0</c:v>
+                  <c:v>8192</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>16384.0</c:v>
+                  <c:v>16384</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>32678.0</c:v>
+                  <c:v>32678</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -923,40 +923,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0.451161</c:v>
+                  <c:v>0.45116099999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.333944</c:v>
+                  <c:v>0.33394400000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.206099</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.176612</c:v>
+                  <c:v>0.17661199999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.128343</c:v>
+                  <c:v>0.12834300000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.098674</c:v>
+                  <c:v>9.8673999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.060589</c:v>
+                  <c:v>6.0588999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.037921</c:v>
+                  <c:v>3.7921000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.032132</c:v>
+                  <c:v>3.2132000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.024051</c:v>
+                  <c:v>2.4050999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.016731</c:v>
+                  <c:v>1.6730999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.01293</c:v>
+                  <c:v>1.2930000000000001E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -979,40 +979,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32.0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>64.0</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>128.0</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>256.0</c:v>
+                  <c:v>256</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>512.0</c:v>
+                  <c:v>512</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1024.0</c:v>
+                  <c:v>1024</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2048.0</c:v>
+                  <c:v>2048</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4096.0</c:v>
+                  <c:v>4096</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8192.0</c:v>
+                  <c:v>8192</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>16384.0</c:v>
+                  <c:v>16384</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>32678.0</c:v>
+                  <c:v>32678</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1030,34 +1030,34 @@
                   <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.333333333333333</c:v>
+                  <c:v>0.33333333333333331</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.285714285714286</c:v>
+                  <c:v>0.2857142857142857</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.222222222222222</c:v>
+                  <c:v>0.22222222222222221</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.181818181818182</c:v>
+                  <c:v>0.18181818181818182</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.166666666666667</c:v>
+                  <c:v>0.16666666666666666</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.153846153846154</c:v>
+                  <c:v>0.15384615384615385</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.142857142857143</c:v>
+                  <c:v>0.14285714285714285</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.133368613171635</c:v>
+                  <c:v>0.13336861317163481</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1074,11 +1074,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="679393336"/>
-        <c:axId val="679318280"/>
+        <c:axId val="112468992"/>
+        <c:axId val="109843520"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="679393336"/>
+        <c:axId val="112468992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1088,7 +1088,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="679318280"/>
+        <c:crossAx val="109843520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1096,7 +1096,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="679318280"/>
+        <c:axId val="109843520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1107,7 +1107,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="679393336"/>
+        <c:crossAx val="112468992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1123,7 +1123,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1165,40 +1165,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32.0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>64.0</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>128.0</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>256.0</c:v>
+                  <c:v>256</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>512.0</c:v>
+                  <c:v>512</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1024.0</c:v>
+                  <c:v>1024</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2048.0</c:v>
+                  <c:v>2048</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4096.0</c:v>
+                  <c:v>4096</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8192.0</c:v>
+                  <c:v>8192</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>16384.0</c:v>
+                  <c:v>16384</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>32678.0</c:v>
+                  <c:v>32678</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1210,40 +1210,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0.564879</c:v>
+                  <c:v>0.56487900000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.45091</c:v>
+                  <c:v>0.45090999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.432415</c:v>
+                  <c:v>0.43241499999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.354833</c:v>
+                  <c:v>0.35483300000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.21978</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.217234</c:v>
+                  <c:v>0.21723400000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.147716</c:v>
+                  <c:v>0.14771599999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.134874</c:v>
+                  <c:v>0.13487399999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.121024</c:v>
+                  <c:v>0.12102400000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.078539</c:v>
+                  <c:v>7.8538999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.07203</c:v>
+                  <c:v>7.2029999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.048683</c:v>
+                  <c:v>4.8682999999999997E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1266,40 +1266,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32.0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>64.0</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>128.0</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>256.0</c:v>
+                  <c:v>256</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>512.0</c:v>
+                  <c:v>512</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1024.0</c:v>
+                  <c:v>1024</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2048.0</c:v>
+                  <c:v>2048</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4096.0</c:v>
+                  <c:v>4096</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8192.0</c:v>
+                  <c:v>8192</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>16384.0</c:v>
+                  <c:v>16384</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>32678.0</c:v>
+                  <c:v>32678</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1320,31 +1320,31 @@
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.428571428571429</c:v>
+                  <c:v>0.42857142857142855</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.375</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.333333333333333</c:v>
+                  <c:v>0.33333333333333331</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.272727272727273</c:v>
+                  <c:v>0.27272727272727271</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.230769230769231</c:v>
+                  <c:v>0.23076923076923078</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.214285714285714</c:v>
+                  <c:v>0.21428571428571427</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.200052919757452</c:v>
+                  <c:v>0.20005291975745224</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1361,11 +1361,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="566048072"/>
-        <c:axId val="607077336"/>
+        <c:axId val="112471040"/>
+        <c:axId val="109845248"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="566048072"/>
+        <c:axId val="112471040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1375,7 +1375,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="607077336"/>
+        <c:crossAx val="109845248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1383,7 +1383,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="607077336"/>
+        <c:axId val="109845248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1394,7 +1394,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="566048072"/>
+        <c:crossAx val="112471040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1410,7 +1410,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1452,40 +1452,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32.0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>64.0</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>128.0</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>256.0</c:v>
+                  <c:v>256</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>512.0</c:v>
+                  <c:v>512</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1024.0</c:v>
+                  <c:v>1024</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2048.0</c:v>
+                  <c:v>2048</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4096.0</c:v>
+                  <c:v>4096</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8192.0</c:v>
+                  <c:v>8192</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>16384.0</c:v>
+                  <c:v>16384</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>32678.0</c:v>
+                  <c:v>32678</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1497,31 +1497,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0.622171</c:v>
+                  <c:v>0.62217100000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.636881</c:v>
+                  <c:v>0.63688100000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.504404</c:v>
+                  <c:v>0.50440399999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.403456</c:v>
+                  <c:v>0.40345599999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.491436</c:v>
+                  <c:v>0.49143599999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.28996</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.255775</c:v>
+                  <c:v>0.25577499999999997</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.220936</c:v>
+                  <c:v>0.22093599999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.188597</c:v>
+                  <c:v>0.18859699999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0.16971</c:v>
@@ -1530,7 +1530,7 @@
                   <c:v>0.135878</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.116696</c:v>
+                  <c:v>0.11669599999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1553,40 +1553,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32.0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>64.0</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>128.0</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>256.0</c:v>
+                  <c:v>256</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>512.0</c:v>
+                  <c:v>512</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1024.0</c:v>
+                  <c:v>1024</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2048.0</c:v>
+                  <c:v>2048</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4096.0</c:v>
+                  <c:v>4096</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8192.0</c:v>
+                  <c:v>8192</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>16384.0</c:v>
+                  <c:v>16384</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>32678.0</c:v>
+                  <c:v>32678</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1598,40 +1598,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.666666666666667</c:v>
+                  <c:v>0.66666666666666663</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.571428571428571</c:v>
+                  <c:v>0.5714285714285714</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.444444444444444</c:v>
+                  <c:v>0.44444444444444442</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.363636363636364</c:v>
+                  <c:v>0.36363636363636365</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.333333333333333</c:v>
+                  <c:v>0.33333333333333331</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.307692307692308</c:v>
+                  <c:v>0.30769230769230771</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.285714285714286</c:v>
+                  <c:v>0.2857142857142857</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.26673722634327</c:v>
+                  <c:v>0.26673722634326963</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1648,11 +1648,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="580711560"/>
-        <c:axId val="566120264"/>
+        <c:axId val="123875328"/>
+        <c:axId val="123929152"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="580711560"/>
+        <c:axId val="123875328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1662,7 +1662,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="566120264"/>
+        <c:crossAx val="123929152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1670,7 +1670,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="566120264"/>
+        <c:axId val="123929152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1681,7 +1681,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="580711560"/>
+        <c:crossAx val="123875328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1697,7 +1697,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1707,16 +1707,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>527050</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:rowOff>6350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1767,16 +1767,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>63500</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>530225</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>53975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>596900</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>463550</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>130175</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1797,16 +1797,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>34925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>508000</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>498475</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2118,12 +2118,12 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:I12"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>16</v>
       </c>
@@ -2131,8 +2131,8 @@
         <v>0.244588</v>
       </c>
       <c r="C1">
-        <f>1/LOG(A1,2)</f>
-        <v>0.25</v>
+        <f>1.5/LOG(A1,2)-0.09</f>
+        <v>0.28500000000000003</v>
       </c>
       <c r="D1">
         <v>0.45116099999999998</v>
@@ -2156,7 +2156,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>32</v>
       </c>
@@ -2164,8 +2164,8 @@
         <v>0.15188499999999999</v>
       </c>
       <c r="C2">
-        <f t="shared" ref="C2:C12" si="0">1/LOG(A2,2)</f>
-        <v>0.2</v>
+        <f t="shared" ref="C2:C12" si="0">1.5/LOG(A2,2)-0.09</f>
+        <v>0.21</v>
       </c>
       <c r="D2">
         <v>0.33394400000000002</v>
@@ -2189,7 +2189,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>64</v>
       </c>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="C3">
         <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
+        <v>0.16</v>
       </c>
       <c r="D3">
         <v>0.206099</v>
@@ -2222,7 +2222,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>128</v>
       </c>
@@ -2231,7 +2231,7 @@
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>0.14285714285714285</v>
+        <v>0.12428571428571428</v>
       </c>
       <c r="D4">
         <v>0.17661199999999999</v>
@@ -2255,7 +2255,7 @@
         <v>0.5714285714285714</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>256</v>
       </c>
@@ -2264,7 +2264,7 @@
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>0.125</v>
+        <v>9.7500000000000003E-2</v>
       </c>
       <c r="D5">
         <v>0.12834300000000001</v>
@@ -2288,7 +2288,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>512</v>
       </c>
@@ -2297,7 +2297,7 @@
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>0.1111111111111111</v>
+        <v>7.6666666666666661E-2</v>
       </c>
       <c r="D6">
         <v>9.8673999999999998E-2</v>
@@ -2321,7 +2321,7 @@
         <v>0.44444444444444442</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1024</v>
       </c>
@@ -2330,7 +2330,7 @@
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.06</v>
       </c>
       <c r="D7">
         <v>6.0588999999999997E-2</v>
@@ -2354,7 +2354,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2048</v>
       </c>
@@ -2363,7 +2363,7 @@
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>9.0909090909090912E-2</v>
+        <v>4.6363636363636357E-2</v>
       </c>
       <c r="D8">
         <v>3.7921000000000003E-2</v>
@@ -2387,7 +2387,7 @@
         <v>0.36363636363636365</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4096</v>
       </c>
@@ -2396,7 +2396,7 @@
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>8.3333333333333329E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="D9">
         <v>3.2132000000000001E-2</v>
@@ -2420,7 +2420,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8192</v>
       </c>
@@ -2429,7 +2429,7 @@
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
-        <v>7.6923076923076927E-2</v>
+        <v>2.5384615384615394E-2</v>
       </c>
       <c r="D10">
         <v>2.4050999999999999E-2</v>
@@ -2453,7 +2453,7 @@
         <v>0.30769230769230771</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>16384</v>
       </c>
@@ -2462,7 +2462,7 @@
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>7.1428571428571425E-2</v>
+        <v>1.714285714285714E-2</v>
       </c>
       <c r="D11">
         <v>1.6730999999999999E-2</v>
@@ -2486,7 +2486,7 @@
         <v>0.2857142857142857</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>32678</v>
       </c>
@@ -2495,7 +2495,7 @@
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>6.6684306585817407E-2</v>
+        <v>1.0026459878726121E-2</v>
       </c>
       <c r="D12">
         <v>1.2930000000000001E-2</v>
@@ -2519,7 +2519,7 @@
         <v>0.26673722634326963</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>0</v>
       </c>

</xml_diff>